<commit_message>
use row.setHeightInPoints to set row height
</commit_message>
<xml_diff>
--- a/src/test/resources/export-goods-with-notice.xlsx
+++ b/src/test/resources/export-goods-with-notice.xlsx
@@ -44,11 +44,14 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
-    <t xml:space="preserve">填写须知：
+    <t>填写须知：
 1、不能增加、删除列；
-3、不能修改灰色单元格；
-2、红色字段为必填字段，黑色字段为选填字段；
-</t>
+2、不能修改灰色单元格；
+3、红色字段为必填字段，黑色字段为选填字段；
+4、删除餐厅编码后再导入，系统会根据ID删除没有餐厅编码的记录；
+5、删除餐厅编码后再导入，系统会根据ID删除没有餐厅编码的记录；
+6、删除餐厅编码后再导入，系统会根据ID删除没有餐厅编码的记录；删除餐厅编码后再导入，系统会根据ID删除没有餐厅编码的记录删除餐厅编码后再导入，系统会根据ID删除没有餐厅编码的记录
+7、删除餐厅编码后再导入，系统会根据ID删除没有餐厅编码的记录；</t>
   </si>
   <si>
     <t>商品名</t>
@@ -386,7 +389,7 @@
     <col min="10" max="10" width="6.0859375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" ht="108.5" customHeight="true">
+    <row r="1" ht="192.0" customHeight="true">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
use  DataFormatter to get number cell value
</commit_message>
<xml_diff>
--- a/src/test/resources/export-goods-with-notice.xlsx
+++ b/src/test/resources/export-goods-with-notice.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>填写须知：
 1、不能增加、删除列；
@@ -84,6 +84,9 @@
     <t>类型</t>
   </si>
   <si>
+    <t>电话</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -102,6 +105,9 @@
     <t>西药</t>
   </si>
   <si>
+    <t>18888888888</t>
+  </si>
+  <si>
     <t>板蓝根</t>
   </si>
   <si>
@@ -112,6 +118,9 @@
   </si>
   <si>
     <t>中药</t>
+  </si>
+  <si>
+    <t>16866666666</t>
   </si>
 </sst>
 </file>
@@ -122,7 +131,7 @@
     <numFmt numFmtId="164" formatCode="yyyy-MM-dd HH:mm:ss"/>
     <numFmt numFmtId="165" formatCode="MM/dd/yyyy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -151,6 +160,11 @@
       <sz val="14.0"/>
       <b val="true"/>
       <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -242,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment wrapText="true" horizontal="left" vertical="top"/>
@@ -277,6 +291,9 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true">
       <alignment wrapText="false"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="false"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true">
       <alignment wrapText="false" horizontal="left"/>
       <protection locked="true"/>
@@ -319,6 +336,10 @@
       <alignment wrapText="false" horizontal="left"/>
       <protection locked="false"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="false" horizontal="left"/>
+      <protection locked="false"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true">
       <alignment wrapText="false" horizontal="left"/>
       <protection locked="true"/>
@@ -354,6 +375,10 @@
       <protection locked="false"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment wrapText="false" horizontal="left"/>
+      <protection locked="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="false" horizontal="left"/>
       <protection locked="false"/>
     </xf>
@@ -371,7 +396,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -387,6 +412,7 @@
     <col min="8" max="8" width="7.41796875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="9" max="9" width="6.2578125" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="6.0859375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="13.79296875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="192.0" customHeight="true">
@@ -425,74 +451,83 @@
       <c r="J2" s="11" t="s">
         <v>10</v>
       </c>
+      <c r="K2" s="12" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="13" t="s">
+      <c r="A3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="B3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="C3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="n" s="17">
+      <c r="D3" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="n" s="18">
         <v>40139.0</v>
       </c>
-      <c r="F3" t="n" s="19">
+      <c r="F3" t="n" s="20">
         <v>40139.0</v>
       </c>
-      <c r="G3" s="20" t="n">
+      <c r="G3" s="21" t="n">
         <v>0.0</v>
       </c>
-      <c r="H3" s="21" t="n">
+      <c r="H3" s="22" t="n">
         <v>1.0E-4</v>
       </c>
-      <c r="I3" s="22" t="n">
-        <v>19.34680938720703</v>
-      </c>
-      <c r="J3" s="23" t="s">
-        <v>16</v>
+      <c r="I3" s="23" t="n">
+        <v>19.350000381469727</v>
+      </c>
+      <c r="J3" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="25" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="n" s="29">
+      <c r="B4" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="n" s="31">
         <v>43617.0</v>
       </c>
-      <c r="F4" t="n" s="31">
+      <c r="F4" t="n" s="33">
         <v>43617.0</v>
       </c>
-      <c r="G4" s="32" t="n">
+      <c r="G4" s="34" t="n">
         <v>135.0</v>
       </c>
-      <c r="H4" s="33" t="n">
+      <c r="H4" s="35" t="n">
         <v>45.56</v>
       </c>
-      <c r="I4" s="34" t="n">
+      <c r="I4" s="36" t="n">
         <v>70.0</v>
       </c>
-      <c r="J4" s="35" t="s">
-        <v>20</v>
+      <c r="J4" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="38" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="decimal" operator="between" sqref="I3:I104" allowBlank="true" errorStyle="stop" showErrorMessage="true">

</xml_diff>

<commit_message>
adjust notice row height
</commit_message>
<xml_diff>
--- a/src/test/resources/export-goods-with-notice.xlsx
+++ b/src/test/resources/export-goods-with-notice.xlsx
@@ -48,9 +48,6 @@
 1、不能增加、删除列；
 2、不能修改灰色单元格；
 3、红色字段为必填字段，黑色字段为选填字段；
-4、删除餐厅编码后再导入，系统会根据ID删除没有餐厅编码的记录；
-5、删除餐厅编码后再导入，系统会根据ID删除没有餐厅编码的记录；
-6、删除餐厅编码后再导入，系统会根据ID删除没有餐厅编码的记录；删除餐厅编码后再导入，系统会根据ID删除没有餐厅编码的记录删除餐厅编码后再导入，系统会根据ID删除没有餐厅编码的记录
 7、删除餐厅编码后再导入，系统会根据ID删除没有餐厅编码的记录；</t>
   </si>
   <si>
@@ -415,7 +412,7 @@
     <col min="11" max="11" width="13.79296875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" ht="192.0" customHeight="true">
+    <row r="1" ht="134.0" customHeight="true">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>